<commit_message>
Add Excel Reader library fix
</commit_message>
<xml_diff>
--- a/Office-Hours/Excel-Rust/report_students.xlsx
+++ b/Office-Hours/Excel-Rust/report_students.xlsx
@@ -25,13 +25,13 @@
     <t>John</t>
   </si>
   <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Jay</t>
+  </si>
+  <si>
     <t>Oscar</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Jay</t>
   </si>
 </sst>
 </file>

</xml_diff>